<commit_message>
css e cronograma alterado
</commit_message>
<xml_diff>
--- a/missao-chamados/materiais/cronograma_chamados.xlsx
+++ b/missao-chamados/materiais/cronograma_chamados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\git_pre\missao-chamados\materiais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B617B89-5C43-4BCD-9F2D-14E7BD1AF64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6BE808-3680-4CAD-955F-C536CF06C90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Item</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Legenda</t>
   </si>
   <si>
-    <t>Revisão: 1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data: </t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
@@ -133,6 +127,18 @@
   </si>
   <si>
     <t xml:space="preserve"> (%) Total (500%)</t>
+  </si>
+  <si>
+    <t>Desenvolver documentação</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>Revisão: 1.2</t>
+  </si>
+  <si>
+    <t>Data:  07/02/2021</t>
   </si>
 </sst>
 </file>
@@ -421,9 +427,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,21 +478,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,36 +504,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,7 +874,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:N7"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -877,7 +883,8 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="5.7109375" customWidth="1"/>
@@ -905,155 +912,155 @@
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="38" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="48" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="32"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="43"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="32"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="43"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="43"/>
+      <c r="B5" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29" t="s">
+      <c r="F6" s="39"/>
+      <c r="G6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="30" t="s">
-        <v>32</v>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="14" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>1</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="25">
         <v>2</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="25">
         <v>3</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <v>4</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="25">
         <v>1</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="30"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
@@ -1061,15 +1068,15 @@
         <v>1</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="32"/>
+        <v>18</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="40"/>
       <c r="G8" s="16">
         <v>44228</v>
       </c>
@@ -1081,11 +1088,11 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="45">
+      <c r="N8" s="28">
         <v>1</v>
       </c>
-      <c r="O8" s="46" t="s">
-        <v>33</v>
+      <c r="O8" s="29" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1094,15 +1101,15 @@
         <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="40"/>
       <c r="G9" s="16">
         <v>44228</v>
       </c>
@@ -1114,11 +1121,11 @@
       <c r="K9" s="22"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="45">
+      <c r="N9" s="28">
         <v>0.3</v>
       </c>
-      <c r="O9" s="46" t="s">
-        <v>34</v>
+      <c r="O9" s="29" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1127,15 +1134,15 @@
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="32"/>
+        <v>24</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="40"/>
       <c r="G10" s="16">
         <v>44228</v>
       </c>
@@ -1147,11 +1154,11 @@
       <c r="K10" s="22"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="45">
+      <c r="N10" s="28">
         <v>0.3</v>
       </c>
-      <c r="O10" s="46" t="s">
-        <v>34</v>
+      <c r="O10" s="29" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1160,15 +1167,15 @@
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="32"/>
+        <v>26</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="40"/>
       <c r="G11" s="16">
         <v>44228</v>
       </c>
@@ -1180,10 +1187,10 @@
       <c r="K11" s="22"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="45">
+      <c r="N11" s="28">
         <v>0</v>
       </c>
-      <c r="O11" s="46"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
@@ -1191,15 +1198,15 @@
         <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="28"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="38"/>
       <c r="G12" s="16">
         <v>44228</v>
       </c>
@@ -1211,10 +1218,10 @@
       <c r="K12" s="22"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="45">
+      <c r="N12" s="28">
         <v>0</v>
       </c>
-      <c r="O12" s="46"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
@@ -1222,47 +1229,59 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="19">
-        <v>44249</v>
-      </c>
-      <c r="H13" s="19">
-        <v>44253</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="46"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="16">
+        <v>44228</v>
+      </c>
+      <c r="H13" s="16">
+        <v>44246</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="28">
+        <v>0</v>
+      </c>
+      <c r="O13" s="29"/>
     </row>
     <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="2">
         <v>7</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="19">
+        <v>44249</v>
+      </c>
+      <c r="H14" s="19">
+        <v>44253</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="22"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="46"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="29"/>
     </row>
     <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
@@ -1271,8 +1290,8 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="1"/>
@@ -1280,8 +1299,8 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="46"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="29"/>
     </row>
     <row r="16" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
@@ -1290,17 +1309,17 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="24"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="48"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
     </row>
     <row r="17" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
@@ -1364,21 +1383,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I6:L6"/>
@@ -1391,6 +1395,21 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Alterado progressão CRUD chamados
</commit_message>
<xml_diff>
--- a/missao-chamados/materiais/cronograma_chamados.xlsx
+++ b/missao-chamados/materiais/cronograma_chamados.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\git_pre\missao-chamados\materiais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JANDERSON\Desktop\projetoIntegrador\ecosystem\missao-chamados\materiais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6BE808-3680-4CAD-955F-C536CF06C90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -126,9 +125,6 @@
     <t>Iniciou o CRUD</t>
   </si>
   <si>
-    <t xml:space="preserve"> (%) Total (500%)</t>
-  </si>
-  <si>
     <t>Desenvolver documentação</t>
   </si>
   <si>
@@ -139,12 +135,18 @@
   </si>
   <si>
     <t>Data:  07/02/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (%) Total (600%)</t>
+  </si>
+  <si>
+    <t>Pendênte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,6 +453,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,45 +506,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,14 +869,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -912,132 +914,132 @@
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="48" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="40"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49"/>
     </row>
     <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="36"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="35" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="36"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="49"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39" t="s">
+      <c r="H6" s="33"/>
+      <c r="I6" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="32" t="s">
+      <c r="N6" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="45" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1059,8 +1061,8 @@
       <c r="M7" s="25">
         <v>1</v>
       </c>
-      <c r="N7" s="41"/>
-      <c r="O7" s="32"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="45"/>
     </row>
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
@@ -1073,10 +1075,10 @@
       <c r="D8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="16">
         <v>44228</v>
       </c>
@@ -1106,10 +1108,10 @@
       <c r="D9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="16">
         <v>44228</v>
       </c>
@@ -1139,10 +1141,10 @@
       <c r="D10" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="16">
         <v>44228</v>
       </c>
@@ -1172,10 +1174,10 @@
       <c r="D11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="40"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="16">
         <v>44228</v>
       </c>
@@ -1190,7 +1192,9 @@
       <c r="N11" s="28">
         <v>0</v>
       </c>
-      <c r="O11" s="29"/>
+      <c r="O11" s="29" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
@@ -1203,10 +1207,10 @@
       <c r="D12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="38"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="16">
         <v>44228</v>
       </c>
@@ -1219,9 +1223,11 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="28">
-        <v>0</v>
-      </c>
-      <c r="O12" s="29"/>
+        <v>0.3</v>
+      </c>
+      <c r="O12" s="29" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
@@ -1229,15 +1235,15 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="38"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="16">
         <v>44228</v>
       </c>
@@ -1265,10 +1271,10 @@
       <c r="D14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="38"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="19">
         <v>44249</v>
       </c>
@@ -1290,8 +1296,8 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="1"/>
@@ -1309,8 +1315,8 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
       <c r="G16" s="27"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1383,6 +1389,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I6:L6"/>
@@ -1395,21 +1416,6 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização cronogramas do projeto
</commit_message>
<xml_diff>
--- a/missao-chamados/materiais/cronograma_chamados.xlsx
+++ b/missao-chamados/materiais/cronograma_chamados.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robes\Desktop\git_pre\missao-chamados\materiais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JANDERSON\Desktop\projetoIntegrador\ecosystem\missao-chamados\materiais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABADE1DF-82F3-41C5-95CE-BCDB2BB5FC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -126,9 +125,6 @@
     <t>Comentários</t>
   </si>
   <si>
-    <t>Todos testarão no insomnia</t>
-  </si>
-  <si>
     <t>Desenvolver documentação</t>
   </si>
   <si>
@@ -138,25 +134,28 @@
     <t xml:space="preserve"> (%) Total (600%)</t>
   </si>
   <si>
-    <t>READ, INSERT, DEL</t>
-  </si>
-  <si>
     <t>TELA LOGIN</t>
   </si>
   <si>
-    <t>EM ANDAMENTO</t>
-  </si>
-  <si>
     <t>Revisão: 1.3</t>
   </si>
   <si>
     <t>Data:  09/02/2021</t>
+  </si>
+  <si>
+    <t>TODOS TESTARÃO NO INSÔMINIA</t>
+  </si>
+  <si>
+    <t>READ,CREATE,UPDATE,DELETE</t>
+  </si>
+  <si>
+    <t>FASE FINAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,21 +467,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,27 +522,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -887,14 +886,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -932,132 +931,132 @@
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="41" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="48" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="35"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="48"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="36"/>
     </row>
     <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="35"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="47" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="47" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="48"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32" t="s">
+      <c r="F6" s="39"/>
+      <c r="G6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32" t="s">
+      <c r="H6" s="39"/>
+      <c r="I6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
       <c r="M6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="44" t="s">
+      <c r="N6" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1079,8 +1078,8 @@
       <c r="M7" s="25">
         <v>1</v>
       </c>
-      <c r="N7" s="33"/>
-      <c r="O7" s="44"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
@@ -1093,10 +1092,10 @@
       <c r="D8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="16">
         <v>44228</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1126,10 +1125,10 @@
       <c r="D9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="16">
         <v>44228</v>
       </c>
@@ -1142,10 +1141,10 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="28">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1159,10 +1158,10 @@
       <c r="D10" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="16">
         <v>44228</v>
       </c>
@@ -1175,10 +1174,10 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="28">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="O10" s="29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1192,10 +1191,10 @@
       <c r="D11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="35"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="16">
         <v>44228</v>
       </c>
@@ -1208,10 +1207,10 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="28">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="O11" s="29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1225,10 +1224,10 @@
       <c r="D12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="38"/>
       <c r="G12" s="16">
         <v>44228</v>
       </c>
@@ -1241,10 +1240,10 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="28">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1253,15 +1252,15 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="16">
         <v>44228</v>
       </c>
@@ -1274,10 +1273,10 @@
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="28">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1291,10 +1290,10 @@
       <c r="D14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="31"/>
+      <c r="F14" s="38"/>
       <c r="G14" s="19">
         <v>44249</v>
       </c>
@@ -1318,8 +1317,8 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="1"/>
@@ -1337,8 +1336,8 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="27"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1346,9 +1345,9 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="49">
+      <c r="N16" s="31">
         <f>SUM(N8:N15)</f>
-        <v>4.25</v>
+        <v>5.75</v>
       </c>
       <c r="O16" s="30"/>
     </row>
@@ -1414,21 +1413,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="I5:O5"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I6:L6"/>
@@ -1441,6 +1425,21 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="I5:O5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>

</xml_diff>